<commit_message>
theca cell tumor --> thecoma
</commit_message>
<xml_diff>
--- a/model performancess.xlsx
+++ b/model performancess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikiv\Desktop\Thesis-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70FBCE77-B5C4-47A4-9E0C-EC9FBDA5F344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3AF604-893C-4E93-A295-14CF8C00DD8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43095" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="first trials for model" sheetId="1" r:id="rId1"/>
@@ -278,12 +278,6 @@
     <t>not correct</t>
   </si>
   <si>
-    <t>https://universe.roboflow.com/vanessas/pcos-image-classification/browse?queryText=class%3ANormal&amp;pageSize=50&amp;startingIndex=0&amp;browseQuery=true</t>
-  </si>
-  <si>
-    <t>https://universe.roboflow.com/elif-5vzyt/ova_canc</t>
-  </si>
-  <si>
     <t>dataset</t>
   </si>
   <si>
@@ -327,6 +321,12 @@
   </si>
   <si>
     <t xml:space="preserve">bening </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://universe.roboflow.com/vanessas/pcos-image-classification/browse?queryText=class%3ANormal&amp;pageSize=50&amp;startingIndex=0&amp;browseQuery=true </t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://universe.roboflow.com/elif-5vzyt/ova_canc </t>
   </si>
 </sst>
 </file>
@@ -336,7 +336,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -392,6 +392,14 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -472,11 +480,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -519,6 +528,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -534,9 +545,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{481FF999-BE42-4641-88B7-5B1969E60D0D}"/>
   </cellStyles>
@@ -554,6 +565,211 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>135255</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>120015</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>588645</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>173355</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C9BC14D-DB90-F8C4-7512-0CE2D3FED782}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10984230" y="6568440"/>
+          <a:ext cx="7768590" cy="2592705"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>184290</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>50940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>18555</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>117615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0EE8A1E-E9B4-80C6-2CE6-CB17B49FE1BF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11033265" y="4327665"/>
+          <a:ext cx="7770495" cy="2600325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>172365</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>105690</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>16155</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>155220</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DAA71B75-59D5-747F-C6CF-164137A0221C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11021340" y="2210715"/>
+          <a:ext cx="7768590" cy="2583180"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>171870</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>36615</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>15660</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>149010</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6519D7B-15AA-DEA3-A5C2-3290A15AD98D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11020845" y="36615"/>
+          <a:ext cx="7768590" cy="2579370"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
@@ -2859,8 +3075,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2898,13 +3114,13 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="18.75" customHeight="1">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="18" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="10" t="s">
@@ -2918,9 +3134,9 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="72">
-      <c r="A3" s="20"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="16"/>
+      <c r="A3" s="22"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="11" t="s">
         <v>10</v>
       </c>
@@ -2950,6 +3166,7 @@
     <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2960,8 +3177,8 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="113" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2974,91 +3191,91 @@
   <sheetData>
     <row r="1" spans="1:8" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="21" t="s">
-        <v>24</v>
+      <c r="F1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="58.2" customHeight="1">
       <c r="A2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>20</v>
+      <c r="B2" s="17" t="s">
+        <v>35</v>
       </c>
       <c r="F2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" t="e" vm="1">
         <v>#VALUE!</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="48.6" customHeight="1">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>21</v>
+      <c r="B3" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G3" t="e" vm="2">
         <v>#VALUE!</v>
       </c>
       <c r="H3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="46.8" customHeight="1">
       <c r="F4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G4" t="e" vm="3">
         <v>#VALUE!</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="59.4" customHeight="1">
       <c r="F5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G5" t="e" vm="4">
         <v>#VALUE!</v>
       </c>
       <c r="H5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="59.4" customHeight="1">
       <c r="F6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G6" t="e" vm="5">
         <v>#VALUE!</v>
       </c>
       <c r="H6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:8">
       <c r="F7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H7" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="72.599999999999994" customHeight="1">
@@ -3069,21 +3286,25 @@
         <v>#VALUE!</v>
       </c>
       <c r="H8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="64.8" customHeight="1">
       <c r="F9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G9" t="e" vm="7">
         <v>#VALUE!</v>
       </c>
       <c r="H9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4028DAD1-2D3C-4D84-B116-279701FD1997}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{4F0BB79C-BA29-4431-99EB-64A90246E347}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3092,8 +3313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6620E8E0-0124-49EA-9B88-DFC4681243D3}">
   <dimension ref="U20:U22"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="148" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20:U22"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="113" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>

<commit_message>
mobilenetv2 done, pictures backed up elsewhere
</commit_message>
<xml_diff>
--- a/model performancess.xlsx
+++ b/model performancess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikiv\Desktop\Thesis-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4377C6-1E7D-4AD8-8229-8224ADFB5378}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0214083-ABF3-4063-87FA-0CB98CDC9D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="first trials for model" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="59">
   <si>
     <t xml:space="preserve">source </t>
   </si>
@@ -393,13 +393,17 @@
   <si>
     <t>DenseNet</t>
   </si>
+  <si>
+    <t>mobilenet</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00%"/>
   </numFmts>
   <fonts count="15">
     <font>
@@ -590,7 +594,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -605,9 +609,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1"/>
@@ -645,9 +646,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -662,6 +660,15 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4443,18 +4450,18 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.5546875" style="12" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.21875" customWidth="1"/>
-    <col min="4" max="4" width="25.88671875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="25.88671875" style="9" customWidth="1"/>
     <col min="5" max="5" width="26.21875" style="5" customWidth="1"/>
     <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -4466,10 +4473,10 @@
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -4480,19 +4487,19 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="18.75" customHeight="1">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="31">
         <v>0.75</v>
       </c>
       <c r="F2" t="s">
@@ -4500,19 +4507,19 @@
       </c>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="31">
         <v>0.77</v>
       </c>
       <c r="F3" t="s">
@@ -4520,11 +4527,22 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="18.75" customHeight="1">
-      <c r="D4" s="11"/>
-      <c r="E4" s="6"/>
+      <c r="A4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="10"/>
+      <c r="E4" s="32">
+        <v>0.7157</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
       <c r="H4" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="E5" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4558,18 +4576,18 @@
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="58.2" customHeight="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F2" t="s">
@@ -4586,7 +4604,7 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="16" t="s">
+      <c r="B3" s="15" t="s">
         <v>32</v>
       </c>
       <c r="F3" t="s">
@@ -4681,16 +4699,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="7"/>
+    <col min="1" max="16384" width="8.88671875" style="6"/>
   </cols>
   <sheetData>
     <row r="20" spans="21:21">
-      <c r="U20" s="7" t="s">
+      <c r="U20" s="6" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" spans="21:21">
-      <c r="U22" s="8" t="s">
+      <c r="U22" s="7" t="s">
         <v>9</v>
       </c>
     </row>
@@ -4719,350 +4737,350 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
     </row>
     <row r="2" spans="1:8">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="21" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
     </row>
-    <row r="3" spans="1:8" s="17" customFormat="1">
-      <c r="A3" s="23">
+    <row r="3" spans="1:8" s="16" customFormat="1">
+      <c r="A3" s="22">
         <v>0</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="22">
         <v>60</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="22">
         <v>64</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="22">
         <v>0.32819999999999999</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <v>12</v>
       </c>
-      <c r="F3" s="23">
+      <c r="F3" s="22">
         <v>5.5539999999999999E-2</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
     </row>
     <row r="4" spans="1:8">
-      <c r="A4" s="23">
+      <c r="A4" s="22">
         <v>1</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="22">
         <v>62.59</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="22">
         <v>60.65</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="22">
         <v>0.32819999999999999</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="22">
         <v>12.23</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="22">
         <v>5.5539999999999999E-2</v>
       </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
     </row>
     <row r="5" spans="1:8">
-      <c r="A5" s="21">
+      <c r="A5" s="20">
         <v>2</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="20">
         <v>76.17</v>
       </c>
-      <c r="C5" s="24">
+      <c r="C5" s="23">
         <v>117.4</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="20">
         <v>0.4264</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="23">
         <v>446.19</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="20">
         <v>2.222E-2</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="20"/>
     </row>
     <row r="6" spans="1:8">
-      <c r="A6" s="21">
+      <c r="A6" s="20">
         <v>3</v>
       </c>
-      <c r="B6" s="21">
+      <c r="B6" s="20">
         <v>77.2</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <v>26.42</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="20">
         <v>0.35260000000000002</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="20">
         <v>19.53</v>
       </c>
-      <c r="F6" s="21">
+      <c r="F6" s="20">
         <v>2.7859999999999999E-2</v>
       </c>
-      <c r="G6" s="21" t="s">
+      <c r="G6" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="20"/>
     </row>
     <row r="7" spans="1:8">
-      <c r="A7" s="21">
+      <c r="A7" s="20">
         <v>4</v>
       </c>
-      <c r="B7" s="21">
+      <c r="B7" s="20">
         <v>77.2</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="20">
         <v>18.55</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="20">
         <v>0.25440000000000002</v>
       </c>
-      <c r="E7" s="21">
+      <c r="E7" s="20">
         <v>18.28</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F7" s="20">
         <v>1.469E-3</v>
       </c>
-      <c r="G7" s="21" t="s">
+      <c r="G7" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="21"/>
+      <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8">
-      <c r="A8" s="21">
+      <c r="A8" s="20">
         <v>5</v>
       </c>
-      <c r="B8" s="21">
+      <c r="B8" s="20">
         <v>78.239999999999995</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <v>61.98</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="20">
         <v>0.30580000000000002</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <v>19.329999999999998</v>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="20">
         <v>3.4819999999999997E-2</v>
       </c>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
     </row>
     <row r="9" spans="1:8">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="21">
+      <c r="B9" s="20">
         <v>70.47</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="20">
         <v>32</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="20">
         <v>0.35260000000000002</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="20">
         <v>20</v>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="20">
         <v>2.768E-2</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
     </row>
     <row r="10" spans="1:8">
-      <c r="A10" s="21"/>
-      <c r="B10" s="21"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
+      <c r="A10" s="20"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
     </row>
     <row r="11" spans="1:8">
-      <c r="A11" s="19" t="s">
+      <c r="A11" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="21"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="20"/>
     </row>
     <row r="12" spans="1:8">
-      <c r="A12" s="19" t="s">
+      <c r="A12" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="21"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
+      <c r="H12" s="20"/>
     </row>
     <row r="13" spans="1:8">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="21"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="20"/>
     </row>
     <row r="14" spans="1:8">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="21"/>
+      <c r="B14" s="24"/>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="20"/>
     </row>
     <row r="15" spans="1:8">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="21"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
+      <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:8">
-      <c r="A16" s="19" t="s">
+      <c r="A16" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
-      <c r="E16" s="25"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="21"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="20"/>
     </row>
     <row r="17" spans="1:8">
-      <c r="A17" s="19" t="s">
+      <c r="A17" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="25"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="21"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="24"/>
+      <c r="G17" s="24"/>
+      <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="B18" s="25"/>
-      <c r="C18" s="25"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="25"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="21"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="24"/>
+      <c r="F18" s="24"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="20"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="21"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
+      <c r="G19" s="24"/>
+      <c r="H19" s="20"/>
     </row>
     <row r="20" spans="1:8">
-      <c r="A20" s="19" t="s">
+      <c r="A20" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="B20" s="25"/>
-      <c r="C20" s="25"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="25"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="21"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="24"/>
+      <c r="E20" s="24"/>
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="20"/>
     </row>
     <row r="21" spans="1:8">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="21"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="21"/>
-      <c r="F22" s="21"/>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="20"/>
+      <c r="H22" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5090,7 +5108,7 @@
       <c r="A1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="20">
+      <c r="B1" s="19">
         <v>0.25</v>
       </c>
     </row>
@@ -5098,7 +5116,7 @@
       <c r="A2" t="s">
         <v>53</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="19">
         <v>0.2</v>
       </c>
     </row>
@@ -5106,7 +5124,7 @@
       <c r="A3" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="19">
         <v>0.3</v>
       </c>
     </row>
@@ -5114,7 +5132,7 @@
       <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>0.15</v>
       </c>
     </row>
@@ -5122,7 +5140,7 @@
       <c r="A5" t="s">
         <v>56</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="19">
         <v>0.1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
backup before i edit all the files
</commit_message>
<xml_diff>
--- a/model performancess.xlsx
+++ b/model performancess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikiv\Desktop\Thesis-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A76543FB-7AB2-46D7-8E2B-8DD578821343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E304CFF3-6B0A-4D4C-8301-398AF8F0C0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="first trials for model" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
   <si>
     <t xml:space="preserve">source </t>
   </si>
@@ -418,6 +418,9 @@
   <si>
     <t>time (m)</t>
   </si>
+  <si>
+    <t>inception v3</t>
+  </si>
 </sst>
 </file>
 
@@ -425,9 +428,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0%"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00%"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00%"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -538,6 +541,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -627,7 +636,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -694,19 +703,28 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -729,7 +747,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-GB"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1993,13 +2011,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>10</xdr:col>
       <xdr:colOff>54899</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>16279</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>363509</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>54899</xdr:rowOff>
@@ -2042,13 +2060,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>125467</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>31692</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>20954</xdr:colOff>
       <xdr:row>14</xdr:row>
       <xdr:rowOff>132831</xdr:rowOff>
@@ -4487,24 +4505,24 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.77734375" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.81640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="42">
+    <row r="1" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -4523,14 +4541,15 @@
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="32" t="s">
         <v>61</v>
       </c>
+      <c r="I1" s="37"/>
     </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
         <v>7</v>
       </c>
@@ -4543,7 +4562,7 @@
       <c r="D2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="31">
+      <c r="E2" s="30">
         <v>0.75</v>
       </c>
       <c r="F2" t="s">
@@ -4552,12 +4571,13 @@
       <c r="G2">
         <v>331.44</v>
       </c>
-      <c r="H2" s="34">
+      <c r="H2" s="33">
         <f>G2/60</f>
         <v>5.524</v>
       </c>
+      <c r="I2" s="33"/>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="29" t="s">
         <v>57</v>
       </c>
@@ -4570,7 +4590,7 @@
       <c r="D3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="31">
+      <c r="E3" s="30">
         <v>0.77449999999999997</v>
       </c>
       <c r="F3" t="s">
@@ -4579,12 +4599,13 @@
       <c r="G3">
         <v>583.88</v>
       </c>
-      <c r="H3" s="34">
+      <c r="H3" s="33">
         <f t="shared" ref="H3:H5" si="0">G3/60</f>
         <v>9.7313333333333336</v>
       </c>
+      <c r="I3" s="33"/>
     </row>
-    <row r="4" spans="1:9" ht="18.75" customHeight="1">
+    <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>58</v>
       </c>
@@ -4597,7 +4618,7 @@
       <c r="D4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="32">
+      <c r="E4" s="31">
         <v>0.80389999999999995</v>
       </c>
       <c r="F4" t="s">
@@ -4606,15 +4627,16 @@
       <c r="G4">
         <v>172.57</v>
       </c>
-      <c r="H4" s="34">
+      <c r="H4" s="33">
         <f t="shared" si="0"/>
         <v>2.8761666666666668</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="33"/>
+      <c r="J4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="12" t="s">
         <v>59</v>
       </c>
@@ -4627,7 +4649,7 @@
       <c r="D5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="31">
+      <c r="E5" s="30">
         <v>0.72550000000000003</v>
       </c>
       <c r="F5" t="s">
@@ -4636,14 +4658,30 @@
       <c r="G5">
         <v>210.58</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="33">
         <f t="shared" si="0"/>
         <v>3.5096666666666669</v>
+      </c>
+      <c r="I5" s="33"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A6" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -4658,15 +4696,15 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="140" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="35" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.44140625" customWidth="1"/>
+    <col min="7" max="7" width="14.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" customHeight="1">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -4680,7 +4718,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="58.2" customHeight="1">
+    <row r="2" spans="1:8" ht="58.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
@@ -4697,7 +4735,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="48.6" customHeight="1">
+    <row r="3" spans="1:8" ht="48.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -4714,7 +4752,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="46.8" customHeight="1">
+    <row r="4" spans="1:8" ht="46.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F4" t="s">
         <v>21</v>
       </c>
@@ -4725,7 +4763,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="59.4" customHeight="1">
+    <row r="5" spans="1:8" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F5" t="s">
         <v>22</v>
       </c>
@@ -4736,7 +4774,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="59.4" customHeight="1">
+    <row r="6" spans="1:8" ht="59.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F6" t="s">
         <v>23</v>
       </c>
@@ -4747,7 +4785,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="F7" t="s">
         <v>24</v>
       </c>
@@ -4755,7 +4793,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="72.599999999999994" customHeight="1">
+    <row r="8" spans="1:8" ht="72.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F8" t="s">
         <v>1</v>
       </c>
@@ -4766,7 +4804,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="64.8" customHeight="1">
+    <row r="9" spans="1:8" ht="64.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="F9" t="s">
         <v>25</v>
       </c>
@@ -4794,17 +4832,17 @@
       <selection activeCell="W23" sqref="W23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="8.88671875" style="6"/>
+    <col min="1" max="16384" width="8.90625" style="6"/>
   </cols>
   <sheetData>
-    <row r="20" spans="21:21">
+    <row r="20" spans="21:21" x14ac:dyDescent="0.35">
       <c r="U20" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="21:21">
+    <row r="22" spans="21:21" x14ac:dyDescent="0.35">
       <c r="U22" s="7" t="s">
         <v>9</v>
       </c>
@@ -4823,29 +4861,29 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.54296875" customWidth="1"/>
     <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" s="30" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="30"/>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>38</v>
       </c>
@@ -4867,7 +4905,7 @@
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
     </row>
-    <row r="3" spans="1:8" s="16" customFormat="1">
+    <row r="3" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="22">
         <v>0</v>
       </c>
@@ -4889,7 +4927,7 @@
       <c r="G3" s="22"/>
       <c r="H3" s="22"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="22">
         <v>1</v>
       </c>
@@ -4911,7 +4949,7 @@
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="20">
         <v>2</v>
       </c>
@@ -4935,7 +4973,7 @@
       </c>
       <c r="H5" s="20"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="20">
         <v>3</v>
       </c>
@@ -4959,7 +4997,7 @@
       </c>
       <c r="H6" s="20"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="20">
         <v>4</v>
       </c>
@@ -4983,7 +5021,7 @@
       </c>
       <c r="H7" s="20"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="20">
         <v>5</v>
       </c>
@@ -5005,7 +5043,7 @@
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="20" t="s">
         <v>40</v>
       </c>
@@ -5027,7 +5065,7 @@
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="20"/>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -5037,7 +5075,7 @@
       <c r="G10" s="20"/>
       <c r="H10" s="20"/>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="18" t="s">
         <v>41</v>
       </c>
@@ -5049,7 +5087,7 @@
       <c r="G11" s="24"/>
       <c r="H11" s="20"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="18" t="s">
         <v>42</v>
       </c>
@@ -5061,7 +5099,7 @@
       <c r="G12" s="24"/>
       <c r="H12" s="20"/>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="18" t="s">
         <v>43</v>
       </c>
@@ -5073,7 +5111,7 @@
       <c r="G13" s="24"/>
       <c r="H13" s="20"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="18" t="s">
         <v>44</v>
       </c>
@@ -5085,7 +5123,7 @@
       <c r="G14" s="24"/>
       <c r="H14" s="20"/>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="18" t="s">
         <v>45</v>
       </c>
@@ -5097,7 +5135,7 @@
       <c r="G15" s="24"/>
       <c r="H15" s="20"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="18" t="s">
         <v>46</v>
       </c>
@@ -5109,7 +5147,7 @@
       <c r="G16" s="24"/>
       <c r="H16" s="20"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17" s="18" t="s">
         <v>47</v>
       </c>
@@ -5121,7 +5159,7 @@
       <c r="G17" s="24"/>
       <c r="H17" s="20"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="18" t="s">
         <v>48</v>
       </c>
@@ -5133,7 +5171,7 @@
       <c r="G18" s="24"/>
       <c r="H18" s="20"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19" s="18" t="s">
         <v>49</v>
       </c>
@@ -5145,7 +5183,7 @@
       <c r="G19" s="24"/>
       <c r="H19" s="20"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" s="18" t="s">
         <v>50</v>
       </c>
@@ -5157,7 +5195,7 @@
       <c r="G20" s="24"/>
       <c r="H20" s="20"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" s="17" t="s">
         <v>51</v>
       </c>
@@ -5169,7 +5207,7 @@
       <c r="G21" s="20"/>
       <c r="H21" s="20"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22" s="20"/>
       <c r="B22" s="20"/>
       <c r="C22" s="20"/>
@@ -5196,12 +5234,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>52</v>
       </c>
@@ -5209,7 +5247,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>53</v>
       </c>
@@ -5217,7 +5255,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -5225,7 +5263,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -5233,7 +5271,7 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>56</v>
       </c>

</xml_diff>

<commit_message>
ensemble nn done 😃
</commit_message>
<xml_diff>
--- a/model performancess.xlsx
+++ b/model performancess.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vikiv\Desktop\Thesis-lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E304CFF3-6B0A-4D4C-8301-398AF8F0C0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AB58D7D-14E2-4DC6-8EA2-3B425F34F2C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="first trials for model" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
   <si>
     <t xml:space="preserve">source </t>
   </si>
@@ -420,6 +420,18 @@
   </si>
   <si>
     <t>inception v3</t>
+  </si>
+  <si>
+    <t>5m 31s</t>
+  </si>
+  <si>
+    <t>9m 43s</t>
+  </si>
+  <si>
+    <t>2m 52s</t>
+  </si>
+  <si>
+    <t>3m 31s</t>
   </si>
 </sst>
 </file>
@@ -548,7 +560,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -563,6 +575,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -636,7 +660,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -700,9 +724,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -713,16 +734,41 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4507,8 +4553,8 @@
   </sheetPr>
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="144" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4541,13 +4587,13 @@
       <c r="F1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="H1" s="32" t="s">
+      <c r="H1" s="31" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="37"/>
+      <c r="I1" s="33"/>
     </row>
     <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
@@ -4562,7 +4608,7 @@
       <c r="D2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="29">
         <v>0.75</v>
       </c>
       <c r="F2" t="s">
@@ -4571,39 +4617,37 @@
       <c r="G2">
         <v>331.44</v>
       </c>
-      <c r="H2" s="33">
-        <f>G2/60</f>
-        <v>5.524</v>
-      </c>
-      <c r="I2" s="33"/>
+      <c r="H2" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="32"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="44">
         <v>0.77449999999999997</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="45">
         <v>583.88</v>
       </c>
-      <c r="H3" s="33">
-        <f t="shared" ref="H3:H5" si="0">G3/60</f>
-        <v>9.7313333333333336</v>
-      </c>
-      <c r="I3" s="33"/>
+      <c r="H3" s="46" t="s">
+        <v>64</v>
+      </c>
+      <c r="I3" s="32"/>
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
@@ -4618,7 +4662,7 @@
       <c r="D4" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="30">
         <v>0.80389999999999995</v>
       </c>
       <c r="F4" t="s">
@@ -4627,11 +4671,10 @@
       <c r="G4">
         <v>172.57</v>
       </c>
-      <c r="H4" s="33">
-        <f t="shared" si="0"/>
-        <v>2.8761666666666668</v>
-      </c>
-      <c r="I4" s="33"/>
+      <c r="H4" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="I4" s="32"/>
       <c r="J4" t="s">
         <v>7</v>
       </c>
@@ -4649,7 +4692,7 @@
       <c r="D5" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="30">
+      <c r="E5" s="29">
         <v>0.72550000000000003</v>
       </c>
       <c r="F5" t="s">
@@ -4658,14 +4701,13 @@
       <c r="G5">
         <v>210.58</v>
       </c>
-      <c r="H5" s="33">
-        <f t="shared" si="0"/>
-        <v>3.5096666666666669</v>
-      </c>
-      <c r="I5" s="33"/>
+      <c r="H5" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="I5" s="32"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
+    <row r="6" spans="1:10" s="39" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="34" t="s">
         <v>62</v>
       </c>
       <c r="B6" s="35" t="s">
@@ -4674,9 +4716,10 @@
       <c r="C6" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="37" t="s">
         <v>15</v>
       </c>
+      <c r="E6" s="38"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4858,7 +4901,7 @@
   <dimension ref="A1:H22"/>
   <sheetViews>
     <sheetView zoomScale="151" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4872,14 +4915,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="34"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
     </row>

</xml_diff>